<commit_message>
remove columns from processed data
</commit_message>
<xml_diff>
--- a/ProcessedMutantLibrary.xlsx
+++ b/ProcessedMutantLibrary.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,65 +374,55 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>CDS strand</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CDS strand</t>
+          <t>e</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>f</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>COG</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>f</t>
+          <t>Locus TAG</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>COG</t>
+          <t>i</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Locus TAG</t>
+          <t>j</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>i</t>
+          <t>Unnamed: 10</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>j</t>
+          <t>Unnamed: 11</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 10</t>
+          <t>Unnamed: 12</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 11</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 12</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 13</t>
         </is>
@@ -443,172 +433,148 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
         <v>6</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>at</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>ar</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="G2" t="n">
         <v>9</v>
       </c>
-      <c r="J2" t="n">
+      <c r="H2" t="n">
         <v>10</v>
       </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" t="n">
         <v>7</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>ag</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>af</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="G3" t="n">
         <v>10</v>
       </c>
-      <c r="J3" t="n">
+      <c r="H3" t="n">
         <v>11</v>
       </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>1 N/A - M</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
       <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>7</v>
-      </c>
-      <c r="F4" t="n">
         <v>8</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>tc</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>rx</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="G4" t="n">
         <v>11</v>
       </c>
-      <c r="J4" t="n">
+      <c r="H4" t="n">
         <v>12</v>
       </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F5" t="n">
         <v>12</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>x42</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>z42</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="G5" t="n">
         <v>15</v>
       </c>
-      <c r="J5" t="n">
+      <c r="H5" t="n">
         <v>16</v>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>abc</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>def</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="K5" t="n">
         <v>14</v>
       </c>
-      <c r="N5" t="n">
+      <c r="L5" t="n">
         <v>13</v>
       </c>
     </row>
@@ -616,93 +582,81 @@
       <c r="A6" t="n">
         <v>9</v>
       </c>
-      <c r="B6" t="n">
-        <v>10</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>1 N/A - M</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>13</v>
+      </c>
       <c r="D6" t="n">
-        <v>12</v>
-      </c>
-      <c r="E6" t="n">
-        <v>13</v>
-      </c>
-      <c r="F6" t="n">
         <v>14</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>stg</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>pdw</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="G6" t="n">
         <v>17</v>
       </c>
-      <c r="J6" t="n">
+      <c r="H6" t="n">
         <v>18</v>
       </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
+        <v>17</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>yt</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>lp</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" t="n">
+        <v>21</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>ftg</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
         <v>15</v>
       </c>
-      <c r="E7" t="n">
-        <v>16</v>
-      </c>
-      <c r="F7" t="n">
-        <v>17</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>yt</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>lp</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>20</v>
-      </c>
-      <c r="J7" t="n">
-        <v>21</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>ftg</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>qwe</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>15</v>
-      </c>
-      <c r="N7" t="n">
+      <c r="L7" t="n">
         <v>16</v>
       </c>
     </row>
@@ -711,130 +665,112 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D8" t="n">
-        <v>17</v>
-      </c>
-      <c r="E8" t="n">
-        <v>18</v>
-      </c>
-      <c r="F8" t="n">
         <v>19</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>bc</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>jk</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="G8" t="n">
         <v>22</v>
       </c>
-      <c r="J8" t="n">
+      <c r="H8" t="n">
         <v>23</v>
       </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>18</v>
-      </c>
-      <c r="E9" t="n">
-        <v>19</v>
-      </c>
-      <c r="F9" t="n">
         <v>20</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>dc</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>mn</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="G9" t="n">
         <v>23</v>
       </c>
-      <c r="J9" t="n">
+      <c r="H9" t="n">
         <v>24</v>
       </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>17</v>
       </c>
       <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" t="n">
+        <v>21</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>lps</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>24</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>ls</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
         <v>18</v>
       </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>19</v>
-      </c>
-      <c r="E10" t="n">
-        <v>20</v>
-      </c>
-      <c r="F10" t="n">
-        <v>21</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>lps</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>24</v>
-      </c>
-      <c r="J10" t="n">
-        <v>25</v>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>ls</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>18</v>
-      </c>
-      <c r="N10" t="n">
+      <c r="L10" t="n">
         <v>19</v>
       </c>
     </row>
@@ -842,43 +778,37 @@
       <c r="A11" t="n">
         <v>18</v>
       </c>
-      <c r="B11" t="n">
-        <v>19</v>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>1 N/A - M</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>21</v>
+      </c>
       <c r="D11" t="n">
-        <v>20</v>
-      </c>
-      <c r="E11" t="n">
-        <v>21</v>
-      </c>
-      <c r="F11" t="n">
         <v>22</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>mnm</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>mbc</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="J11" t="n">
+      <c r="H11" t="n">
         <v>32</v>
       </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -893,8 +823,6 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>